<commit_message>
add Integration tests Excel.setcell
Tests for Integers and Doubles.
</commit_message>
<xml_diff>
--- a/xill-runtime/src/test/resources/testresources/excel/getCellWorkbook.xlsx
+++ b/xill-runtime/src/test/resources/testresources/excel/getCellWorkbook.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geert\Code\xillio\xill-package\src\test\resources\testresources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sander\Documents\xillprojects\xill-platform\xill-runtime\src\test\resources\testresources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7968" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="integer" sheetId="1" r:id="rId1"/>
+    <sheet name="double" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -23,15 +24,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Integer test</t>
+  </si>
+  <si>
+    <t>double test</t>
+  </si>
+  <si>
+    <t>This should convert to a double since it is bigger than max long</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,12 +75,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -75,9 +97,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -115,7 +137,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -221,7 +243,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -371,24 +393,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>12345678910</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>-12345678910</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1000.0005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>-1000.0005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>12345678910.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>-12345678910.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>9.5233720368547697E+18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
check values smaller than Long.MIN_VALUE
Added Integration test for it.
</commit_message>
<xml_diff>
--- a/xill-runtime/src/test/resources/testresources/excel/getCellWorkbook.xlsx
+++ b/xill-runtime/src/test/resources/testresources/excel/getCellWorkbook.xlsx
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,6 +569,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>-9.5233720368547697E+18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>